<commit_message>
small title change update
added a word in the title to make things clearer
</commit_message>
<xml_diff>
--- a/Testing/Sprint 3 Tests/SR_38.1.1.xlsx
+++ b/Testing/Sprint 3 Tests/SR_38.1.1.xlsx
@@ -83,9 +83,6 @@
     <t>SR_38.1</t>
   </si>
   <si>
-    <t>[Sub-story] Join Group</t>
-  </si>
-  <si>
     <t>As a student, I want to be able to join other study groups so I can study the same topic</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
       </rPr>
       <t>STUDYRING - Sprint 3 Testing</t>
     </r>
+  </si>
+  <si>
+    <t>[Sub-story] Join Public Group</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -828,7 +828,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -863,7 +863,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>13</v>
@@ -877,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -910,14 +910,14 @@
     </row>
     <row r="8" spans="1:8" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>0</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>15</v>
@@ -944,7 +944,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>